<commit_message>
change in the server speed comp.
</commit_message>
<xml_diff>
--- a/test_data/server_speed_comparison.xlsx
+++ b/test_data/server_speed_comparison.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC857D20-AAFE-426A-8F4F-C6224B69CD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E4D9D5-DE15-4CFF-BB4C-52C4E00D14EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="540" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="desktop(6-3-24)" sheetId="1" r:id="rId1"/>
+    <sheet name="desktop(12th Mar - 24)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>nordvpn</t>
   </si>
@@ -61,6 +62,36 @@
   </si>
   <si>
     <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>ping(ms)</t>
+  </si>
+  <si>
+    <t>Serbia(Belgrade)</t>
+  </si>
+  <si>
+    <t>speedtest.net</t>
+  </si>
+  <si>
+    <t>Colombia(Bogota)</t>
+  </si>
+  <si>
+    <t>Chile(Santiago)</t>
+  </si>
+  <si>
+    <t>Denmark(Copenhegen)</t>
+  </si>
+  <si>
+    <t>Greece(Athenes)</t>
+  </si>
+  <si>
+    <t>Honkong</t>
+  </si>
+  <si>
+    <t>Finland</t>
   </si>
 </sst>
 </file>
@@ -84,12 +115,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -122,6 +159,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -406,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,4 +578,260 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70876F9D-7AB4-4BAB-A9FF-6EC889FD86F5}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="19.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7">
+        <v>5.67</v>
+      </c>
+      <c r="C3" s="7">
+        <v>51.85</v>
+      </c>
+      <c r="D3" s="7">
+        <v>323</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.37</v>
+      </c>
+      <c r="F3" s="7">
+        <v>66.37</v>
+      </c>
+      <c r="G3" s="7">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="C4" s="2">
+        <v>62.47</v>
+      </c>
+      <c r="D4" s="2">
+        <v>326</v>
+      </c>
+      <c r="E4" s="2">
+        <v>37.6</v>
+      </c>
+      <c r="F4" s="3">
+        <v>46.97</v>
+      </c>
+      <c r="G4" s="2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7">
+        <v>68.569999999999993</v>
+      </c>
+      <c r="C5" s="7">
+        <v>48.32</v>
+      </c>
+      <c r="D5" s="7">
+        <v>331</v>
+      </c>
+      <c r="E5" s="7">
+        <v>30.67</v>
+      </c>
+      <c r="F5" s="8">
+        <v>6.45</v>
+      </c>
+      <c r="G5" s="7">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>15.21</v>
+      </c>
+      <c r="C6" s="2">
+        <v>14.44</v>
+      </c>
+      <c r="D6" s="2">
+        <v>584</v>
+      </c>
+      <c r="E6" s="2">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7">
+        <v>82.84</v>
+      </c>
+      <c r="C7" s="7">
+        <v>62.67</v>
+      </c>
+      <c r="D7" s="7">
+        <v>221</v>
+      </c>
+      <c r="E7" s="7">
+        <v>79.83</v>
+      </c>
+      <c r="F7" s="8">
+        <v>22.63</v>
+      </c>
+      <c r="G7" s="7">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2">
+        <v>79.58</v>
+      </c>
+      <c r="C8" s="2">
+        <v>50.48</v>
+      </c>
+      <c r="D8" s="2">
+        <v>235</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7.08</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7.44</v>
+      </c>
+      <c r="G8" s="2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7">
+        <v>83.78</v>
+      </c>
+      <c r="C9" s="7">
+        <v>73.180000000000007</v>
+      </c>
+      <c r="D9" s="7">
+        <v>100</v>
+      </c>
+      <c r="E9" s="7">
+        <v>78.86</v>
+      </c>
+      <c r="F9" s="7">
+        <v>42.34</v>
+      </c>
+      <c r="G9" s="7">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2">
+        <v>83.29</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44.06</v>
+      </c>
+      <c r="D10" s="2">
+        <v>238</v>
+      </c>
+      <c r="E10" s="2">
+        <v>12.16</v>
+      </c>
+      <c r="F10" s="2">
+        <v>30.73</v>
+      </c>
+      <c r="G10" s="2">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>